<commit_message>
add 3LDK_07 data and rename some files
</commit_message>
<xml_diff>
--- a/SIGVerse/dataset/similar/3LDK/3LDK_07/position/3LDK_7_position.xlsx
+++ b/SIGVerse/dataset/similar/3LDK/3LDK_07/position/3LDK_7_position.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akira\Dropbox\SpCoNavi\CoRL\dataset\similar\dataset_C\3LDK_7\position\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akira\Dropbox\SpCoSLAM\SpCoTMHP\SIGVerse\dataset\similar\3LDK\3LDK_07\position\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="3LDK_7_position" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -629,8 +629,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -738,7 +744,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.7296387569874377E-2"/>
+          <c:y val="0.10378452861558569"/>
+          <c:w val="0.92891226382961667"/>
+          <c:h val="0.86445783188056979"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -780,10 +796,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'3LDK_7_position'!$D$2:$D$151</c:f>
+              <c:f>'3LDK_7_position'!$D$2:$D$166</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="150"/>
+                <c:ptCount val="165"/>
                 <c:pt idx="0">
                   <c:v>2.0099999999999998</c:v>
                 </c:pt>
@@ -875,49 +891,49 @@
                   <c:v>3.01</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.86</c:v>
+                  <c:v>-3.86</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.88</c:v>
+                  <c:v>-3.298</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.98</c:v>
+                  <c:v>-2.786</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.12</c:v>
+                  <c:v>-2.2660000000000005</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.2699999999999996</c:v>
+                  <c:v>-1.708</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.28</c:v>
+                  <c:v>-1.07</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.51</c:v>
+                  <c:v>-0.45100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.76</c:v>
+                  <c:v>0.23799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.88</c:v>
+                  <c:v>0.97599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.92</c:v>
+                  <c:v>1.722</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.26</c:v>
+                  <c:v>2.63</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.12</c:v>
+                  <c:v>3.3280000000000003</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.97</c:v>
+                  <c:v>3.976</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.33</c:v>
+                  <c:v>4.1135000000000002</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>4.71</c:v>
@@ -1233,16 +1249,61 @@
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>-4.38</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>-4.78</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>-5.18</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>-5.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>-5.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>-4.66</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>-4.68</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>-4.46</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>-4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>-5.2</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>-5.36</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>-4.9600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>-4.78</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>-4.88</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>-4.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3LDK_7_position'!$C$2:$C$151</c:f>
+              <c:f>'3LDK_7_position'!$C$2:$C$166</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="150"/>
+                <c:ptCount val="165"/>
                 <c:pt idx="0">
                   <c:v>2.48</c:v>
                 </c:pt>
@@ -1334,49 +1395,49 @@
                   <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.19</c:v>
+                  <c:v>-4.38</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.39</c:v>
+                  <c:v>-4.78</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.59</c:v>
+                  <c:v>-5.18</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.65</c:v>
+                  <c:v>-5.3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.5099999999999998</c:v>
+                  <c:v>-5.0199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.33</c:v>
+                  <c:v>-4.66</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.34</c:v>
+                  <c:v>-4.68</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.23</c:v>
+                  <c:v>-4.46</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.4300000000000002</c:v>
+                  <c:v>-4.8600000000000003</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.6</c:v>
+                  <c:v>-5.2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.68</c:v>
+                  <c:v>-5.36</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.48</c:v>
+                  <c:v>-4.96</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.39</c:v>
+                  <c:v>-4.78</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.44</c:v>
+                  <c:v>-4.88</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.44</c:v>
+                  <c:v>-4.88</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>1.88</c:v>
@@ -1692,6 +1753,51 @@
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>3.01</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>-4.0327999999999999</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>-3.48204</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>-2.98028</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>-2.4706800000000002</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>-1.92384</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>-1.2986</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>-0.69198000000000004</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>-1.6760000000000025E-2</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.70648</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>1.4375599999999999</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2.3273999999999999</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>3.0114400000000003</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>3.6464799999999999</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>3.7812299999999999</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>4.0620000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1706,11 +1812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118207336"/>
-        <c:axId val="118206944"/>
+        <c:axId val="456519616"/>
+        <c:axId val="456521968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118207336"/>
+        <c:axId val="456519616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1767,12 +1873,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118206944"/>
+        <c:crossAx val="456521968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118206944"/>
+        <c:axId val="456521968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1829,7 +1935,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118207336"/>
+        <c:crossAx val="456519616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2444,8 +2550,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>64977</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>29571</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2454,7 +2560,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -2462,14 +2568,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect b="3620"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4591051" y="581025"/>
-          <a:ext cx="5075126" cy="4763496"/>
+          <a:ext cx="5075126" cy="4591050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2480,16 +2585,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:colOff>523877</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2506,6 +2611,1144 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>481013</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>33340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>576263</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>100015</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="11919" t="17296" r="23965" b="20097"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="5400000">
+          <a:off x="10096500" y="533403"/>
+          <a:ext cx="4867275" cy="4895850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="円/楕円 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10487025" y="1743075"/>
+          <a:ext cx="238125" cy="2876550"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>481012</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>128590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>23815</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="円/楕円 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="12389643" y="3136109"/>
+          <a:ext cx="238125" cy="3481387"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="角丸四角形吹き出し 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13763625" y="1104900"/>
+          <a:ext cx="1295400" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -20349"/>
+            <a:gd name="adj2" fmla="val 214396"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>バスルームを消す</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="角丸四角形吹き出し 33"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8934450" y="2743200"/>
+          <a:ext cx="1295400" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 75239"/>
+            <a:gd name="adj2" fmla="val 28285"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>みなみ　ろうか</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609799</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>153213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190699</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>62873</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="上下矢印 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="550227">
+          <a:off x="11582599" y="3239313"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>485973</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19863</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66873</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>100973</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="上下矢印 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="20351554">
+          <a:off x="12830373" y="3277413"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>485973</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>29388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66873</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>110498</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="上下矢印 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="550227">
+          <a:off x="12830373" y="2086788"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>209072</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>143633</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>475772</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>61793</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="上下矢印 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2301349">
+          <a:off x="13239272" y="2372483"/>
+          <a:ext cx="266700" cy="603960"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>142167</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>109998</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>339432</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>33798</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="上下矢印 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="3423099">
+          <a:off x="13480550" y="2373565"/>
+          <a:ext cx="266700" cy="883065"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>149946</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>2455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>59606</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>97705</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="上下矢印 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="13344526" y="2924175"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>499916</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>147784</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>71584</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="上下矢印 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5199671">
+          <a:off x="10951296" y="2212254"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>4911</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="上下矢印 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="550227">
+          <a:off x="11306176" y="4381501"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>4911</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="上下矢印 42"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="550227">
+          <a:off x="13801726" y="4381501"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>369020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>59606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>278680</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>154856</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="上下矢印 43"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="12192000" y="2638426"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>214460</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="上下矢印 45"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="3174234">
+          <a:off x="10756180" y="1597745"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="角丸四角形吹き出し 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11830050" y="5219700"/>
+          <a:ext cx="1295400" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 4651"/>
+            <a:gd name="adj2" fmla="val -138382"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ひがし　ろうか</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="乗算記号 46"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13744575" y="1743075"/>
+          <a:ext cx="733425" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 7036"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266898</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>105589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>533598</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>15249</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="上下矢印 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="20351554">
+          <a:off x="10553898" y="4391839"/>
+          <a:ext cx="266700" cy="595460"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2774,10 +4017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F151"/>
+  <dimension ref="A1:P166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3102,7 +4345,7 @@
         <v>-0.29670825290000002</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3122,7 +4365,7 @@
         <v>0.91340342409999997</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3142,7 +4385,7 @@
         <v>0.95105651629999999</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3162,7 +4405,7 @@
         <v>0.91761593900000005</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3182,7 +4425,7 @@
         <v>0.89462263870000003</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3202,7 +4445,7 @@
         <v>0.8738570913</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3222,7 +4465,7 @@
         <v>0.99182777580000003</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3242,7 +4485,7 @@
         <v>0.99185002820000001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3262,7 +4505,7 @@
         <v>0.97313870670000002</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3282,7 +4525,7 @@
         <v>0.97644687249999995</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3302,7 +4545,7 @@
         <v>0.99801575419999999</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3322,7 +4565,7 @@
         <v>0.98020211950000002</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3342,7 +4585,7 @@
         <v>0.99686231599999997</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3362,7 +4605,7 @@
         <v>0.99989507639999997</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3382,7 +4625,7 @@
         <v>0.99827074380000003</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3402,18 +4645,18 @@
         <v>0.9698720153</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
         <v>-129.88999999999999</v>
       </c>
       <c r="C32">
-        <v>2.19</v>
-      </c>
-      <c r="D32">
-        <v>3.86</v>
+        <v>-4.38</v>
+      </c>
+      <c r="D32" s="1">
+        <v>-3.86</v>
       </c>
       <c r="E32">
         <v>0.76727709420000001</v>
@@ -3421,19 +4664,39 @@
       <c r="F32">
         <v>0.64131572619999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33">
+      <c r="H32">
+        <v>2.19</v>
+      </c>
+      <c r="I32">
+        <v>3.86</v>
+      </c>
+      <c r="K32">
+        <v>-2</v>
+      </c>
+      <c r="L32">
+        <v>-1</v>
+      </c>
+      <c r="N32">
+        <f>H32*K32</f>
+        <v>-4.38</v>
+      </c>
+      <c r="O32">
+        <f>I32*L32</f>
+        <v>-3.86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
         <v>-120.45</v>
       </c>
       <c r="C33">
-        <v>2.39</v>
-      </c>
-      <c r="D33">
-        <v>3.88</v>
+        <v>-4.78</v>
+      </c>
+      <c r="D33" s="1">
+        <v>-3.298</v>
       </c>
       <c r="E33">
         <v>0.86207174310000001</v>
@@ -3441,19 +4704,39 @@
       <c r="F33">
         <v>0.50678625649999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34">
+      <c r="H33">
+        <v>2.39</v>
+      </c>
+      <c r="I33">
+        <v>3.88</v>
+      </c>
+      <c r="K33">
+        <v>-2</v>
+      </c>
+      <c r="L33">
+        <v>-0.85</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ref="N33:N46" si="0">H33*K33</f>
+        <v>-4.78</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ref="O33:O46" si="1">I33*L33</f>
+        <v>-3.298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
         <v>-116.16</v>
       </c>
       <c r="C34">
-        <v>2.59</v>
-      </c>
-      <c r="D34">
-        <v>3.98</v>
+        <v>-5.18</v>
+      </c>
+      <c r="D34" s="1">
+        <v>-2.786</v>
       </c>
       <c r="E34">
         <v>0.89756638020000001</v>
@@ -3461,19 +4744,39 @@
       <c r="F34">
         <v>0.44087934070000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35">
+      <c r="H34">
+        <v>2.59</v>
+      </c>
+      <c r="I34">
+        <v>3.98</v>
+      </c>
+      <c r="K34">
+        <v>-2</v>
+      </c>
+      <c r="L34">
+        <v>-0.7</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>-5.18</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="1"/>
+        <v>-2.786</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
         <v>-106.12</v>
       </c>
       <c r="C35">
-        <v>2.65</v>
-      </c>
-      <c r="D35">
-        <v>4.12</v>
+        <v>-5.3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>-2.2660000000000005</v>
       </c>
       <c r="E35">
         <v>0.96068229459999999</v>
@@ -3481,19 +4784,39 @@
       <c r="F35">
         <v>0.27765001160000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36">
+      <c r="H35">
+        <v>2.65</v>
+      </c>
+      <c r="I35">
+        <v>4.12</v>
+      </c>
+      <c r="K35">
+        <v>-2</v>
+      </c>
+      <c r="L35">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>-5.3</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="1"/>
+        <v>-2.2660000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
         <v>-127.28</v>
       </c>
       <c r="C36">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="D36">
-        <v>4.2699999999999996</v>
+        <v>-5.0199999999999996</v>
+      </c>
+      <c r="D36" s="1">
+        <v>-1.708</v>
       </c>
       <c r="E36">
         <v>0.79568496219999996</v>
@@ -3501,19 +4824,39 @@
       <c r="F36">
         <v>0.60571069070000005</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37">
+      <c r="H36">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I36">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="K36">
+        <v>-2</v>
+      </c>
+      <c r="L36">
+        <v>-0.4</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>-5.0199999999999996</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="1"/>
+        <v>-1.708</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
         <v>-147.02000000000001</v>
       </c>
       <c r="C37">
-        <v>2.33</v>
-      </c>
-      <c r="D37">
-        <v>4.28</v>
+        <v>-4.66</v>
+      </c>
+      <c r="D37" s="1">
+        <v>-1.07</v>
       </c>
       <c r="E37">
         <v>0.54434625059999997</v>
@@ -3521,19 +4864,39 @@
       <c r="F37">
         <v>0.83886063170000003</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38">
+      <c r="H37">
+        <v>2.33</v>
+      </c>
+      <c r="I37">
+        <v>4.28</v>
+      </c>
+      <c r="K37">
+        <v>-2</v>
+      </c>
+      <c r="L37">
+        <v>-0.25</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>-4.66</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="1"/>
+        <v>-1.07</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
         <v>-158.72</v>
       </c>
       <c r="C38">
-        <v>2.34</v>
-      </c>
-      <c r="D38">
-        <v>4.51</v>
+        <v>-4.68</v>
+      </c>
+      <c r="D38" s="1">
+        <v>-0.45100000000000001</v>
       </c>
       <c r="E38">
         <v>0.36292598679999999</v>
@@ -3541,19 +4904,39 @@
       <c r="F38">
         <v>0.93181796939999995</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39">
+      <c r="H38">
+        <v>2.34</v>
+      </c>
+      <c r="I38">
+        <v>4.51</v>
+      </c>
+      <c r="K38">
+        <v>-2</v>
+      </c>
+      <c r="L38">
+        <v>-0.1</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>-4.68</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="1"/>
+        <v>-0.45100000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
         <v>174.86</v>
       </c>
       <c r="C39">
-        <v>2.23</v>
-      </c>
-      <c r="D39">
-        <v>4.76</v>
+        <v>-4.46</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.23799999999999999</v>
       </c>
       <c r="E39">
         <v>-8.9589642999999997E-2</v>
@@ -3561,19 +4944,39 @@
       <c r="F39">
         <v>0.99597876279999997</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40">
+      <c r="H39">
+        <v>2.23</v>
+      </c>
+      <c r="I39">
+        <v>4.76</v>
+      </c>
+      <c r="K39">
+        <v>-2</v>
+      </c>
+      <c r="L39">
+        <v>0.05</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>-4.46</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="1"/>
+        <v>0.23799999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
         <v>153.9</v>
       </c>
       <c r="C40">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="D40">
-        <v>4.88</v>
+        <v>-4.8600000000000003</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.97599999999999998</v>
       </c>
       <c r="E40">
         <v>-0.43993916989999998</v>
@@ -3581,19 +4984,39 @@
       <c r="F40">
         <v>0.89802757580000003</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41">
+      <c r="H40">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="I40">
+        <v>4.88</v>
+      </c>
+      <c r="K40">
+        <v>-2</v>
+      </c>
+      <c r="L40">
+        <v>0.2</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="0"/>
+        <v>-4.8600000000000003</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="1"/>
+        <v>0.97599999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
         <v>148.27000000000001</v>
       </c>
       <c r="C41">
-        <v>2.6</v>
-      </c>
-      <c r="D41">
-        <v>4.92</v>
+        <v>-5.2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1.722</v>
       </c>
       <c r="E41">
         <v>-0.52591706270000005</v>
@@ -3601,19 +5024,39 @@
       <c r="F41">
         <v>0.85053585649999996</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42">
+      <c r="H41">
+        <v>2.6</v>
+      </c>
+      <c r="I41">
+        <v>4.92</v>
+      </c>
+      <c r="K41">
+        <v>-2</v>
+      </c>
+      <c r="L41">
+        <v>0.35</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="0"/>
+        <v>-5.2</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="1"/>
+        <v>1.722</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
         <v>126.36</v>
       </c>
       <c r="C42">
-        <v>2.68</v>
-      </c>
-      <c r="D42">
-        <v>5.26</v>
+        <v>-5.36</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2.63</v>
       </c>
       <c r="E42">
         <v>-0.8053078857</v>
@@ -3621,19 +5064,39 @@
       <c r="F42">
         <v>0.59285682019999997</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43">
+      <c r="H42">
+        <v>2.68</v>
+      </c>
+      <c r="I42">
+        <v>5.26</v>
+      </c>
+      <c r="K42">
+        <v>-2</v>
+      </c>
+      <c r="L42">
+        <v>0.5</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="0"/>
+        <v>-5.36</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="1"/>
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
         <v>148.01</v>
       </c>
       <c r="C43">
-        <v>2.48</v>
-      </c>
-      <c r="D43">
-        <v>5.12</v>
+        <v>-4.96</v>
+      </c>
+      <c r="D43" s="1">
+        <v>3.3280000000000003</v>
       </c>
       <c r="E43">
         <v>-0.52977124379999996</v>
@@ -3641,19 +5104,39 @@
       <c r="F43">
         <v>0.8481405716</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44">
+      <c r="H43">
+        <v>2.48</v>
+      </c>
+      <c r="I43">
+        <v>5.12</v>
+      </c>
+      <c r="K43">
+        <v>-2</v>
+      </c>
+      <c r="L43">
+        <v>0.65</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="0"/>
+        <v>-4.96</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="1"/>
+        <v>3.3280000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
         <v>172.23</v>
       </c>
       <c r="C44">
-        <v>2.39</v>
-      </c>
-      <c r="D44">
-        <v>4.97</v>
+        <v>-4.78</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3.976</v>
       </c>
       <c r="E44">
         <v>-0.13519679949999999</v>
@@ -3661,19 +5144,39 @@
       <c r="F44">
         <v>0.99081876520000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45">
+      <c r="H44">
+        <v>2.39</v>
+      </c>
+      <c r="I44">
+        <v>4.97</v>
+      </c>
+      <c r="K44">
+        <v>-2</v>
+      </c>
+      <c r="L44">
+        <v>0.8</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="0"/>
+        <v>-4.78</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="1"/>
+        <v>3.976</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
         <v>-140.24</v>
       </c>
       <c r="C45">
-        <v>2.44</v>
-      </c>
-      <c r="D45">
-        <v>4.33</v>
+        <v>-4.88</v>
+      </c>
+      <c r="D45" s="1">
+        <v>4.1135000000000002</v>
       </c>
       <c r="E45">
         <v>0.6395731805</v>
@@ -3681,19 +5184,39 @@
       <c r="F45">
         <v>0.76873021720000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46">
+      <c r="H45">
+        <v>2.44</v>
+      </c>
+      <c r="I45">
+        <v>4.33</v>
+      </c>
+      <c r="K45">
+        <v>-2</v>
+      </c>
+      <c r="L45">
+        <v>0.95</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="0"/>
+        <v>-4.88</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="1"/>
+        <v>4.1135000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
         <v>-95.49</v>
       </c>
       <c r="C46">
-        <v>2.44</v>
-      </c>
-      <c r="D46">
-        <v>4</v>
+        <v>-4.88</v>
+      </c>
+      <c r="D46" s="1">
+        <v>4.4000000000000004</v>
       </c>
       <c r="E46">
         <v>0.99541291139999999</v>
@@ -3701,8 +5224,28 @@
       <c r="F46">
         <v>9.5672021699999998E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="H46">
+        <v>2.44</v>
+      </c>
+      <c r="I46">
+        <v>4</v>
+      </c>
+      <c r="K46">
+        <v>-2</v>
+      </c>
+      <c r="L46">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="0"/>
+        <v>-4.88</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3722,7 +5265,7 @@
         <v>-0.77582621240000005</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>46</v>
       </c>
@@ -5662,7 +7205,7 @@
         <v>0.21047175979999999</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A145">
         <v>143</v>
       </c>
@@ -5682,7 +7225,7 @@
         <v>0.2910361668</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A146">
         <v>144</v>
       </c>
@@ -5702,7 +7245,7 @@
         <v>0.32853697720000002</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A147">
         <v>145</v>
       </c>
@@ -5722,7 +7265,7 @@
         <v>0.40705550579999999</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A148">
         <v>146</v>
       </c>
@@ -5742,7 +7285,7 @@
         <v>0.70488185390000002</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A149">
         <v>147</v>
       </c>
@@ -5762,7 +7305,7 @@
         <v>0.85264016440000001</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A150">
         <v>148</v>
       </c>
@@ -5782,7 +7325,7 @@
         <v>0.96159773299999995</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A151">
         <v>149</v>
       </c>
@@ -5802,9 +7345,640 @@
         <v>0.96529052920000002</v>
       </c>
     </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A152" s="2">
+        <v>150</v>
+      </c>
+      <c r="C152" s="2">
+        <v>-4.0327999999999999</v>
+      </c>
+      <c r="D152" s="2">
+        <v>-4.38</v>
+      </c>
+      <c r="I152">
+        <v>-3.86</v>
+      </c>
+      <c r="J152">
+        <v>-5.4749999999999996</v>
+      </c>
+      <c r="K152">
+        <v>0.8</v>
+      </c>
+      <c r="L152">
+        <f>J152*K152</f>
+        <v>-4.38</v>
+      </c>
+      <c r="M152">
+        <v>0.98</v>
+      </c>
+      <c r="N152">
+        <f>I152*M152</f>
+        <v>-3.7827999999999999</v>
+      </c>
+      <c r="O152">
+        <v>-0.25</v>
+      </c>
+      <c r="P152">
+        <f>N152+O152</f>
+        <v>-4.0327999999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A153" s="2">
+        <v>151</v>
+      </c>
+      <c r="C153" s="2">
+        <v>-3.48204</v>
+      </c>
+      <c r="D153" s="2">
+        <v>-4.78</v>
+      </c>
+      <c r="I153">
+        <v>-3.298</v>
+      </c>
+      <c r="J153">
+        <v>-5.9750000000000005</v>
+      </c>
+      <c r="K153">
+        <v>0.8</v>
+      </c>
+      <c r="L153">
+        <f t="shared" ref="L153:L166" si="2">J153*K153</f>
+        <v>-4.78</v>
+      </c>
+      <c r="M153">
+        <v>0.98</v>
+      </c>
+      <c r="N153">
+        <f t="shared" ref="N153:N166" si="3">I153*M153</f>
+        <v>-3.23204</v>
+      </c>
+      <c r="O153">
+        <v>-0.25</v>
+      </c>
+      <c r="P153">
+        <f t="shared" ref="P153:P166" si="4">N153+O153</f>
+        <v>-3.48204</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A154" s="2">
+        <v>152</v>
+      </c>
+      <c r="C154" s="2">
+        <v>-2.98028</v>
+      </c>
+      <c r="D154" s="2">
+        <v>-5.18</v>
+      </c>
+      <c r="I154">
+        <v>-2.786</v>
+      </c>
+      <c r="J154">
+        <v>-6.4749999999999996</v>
+      </c>
+      <c r="K154">
+        <v>0.8</v>
+      </c>
+      <c r="L154">
+        <f t="shared" si="2"/>
+        <v>-5.18</v>
+      </c>
+      <c r="M154">
+        <v>0.98</v>
+      </c>
+      <c r="N154">
+        <f t="shared" si="3"/>
+        <v>-2.73028</v>
+      </c>
+      <c r="O154">
+        <v>-0.25</v>
+      </c>
+      <c r="P154">
+        <f t="shared" si="4"/>
+        <v>-2.98028</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A155" s="2">
+        <v>153</v>
+      </c>
+      <c r="C155" s="2">
+        <v>-2.4706800000000002</v>
+      </c>
+      <c r="D155" s="2">
+        <v>-5.3000000000000007</v>
+      </c>
+      <c r="I155">
+        <v>-2.2660000000000005</v>
+      </c>
+      <c r="J155">
+        <v>-6.625</v>
+      </c>
+      <c r="K155">
+        <v>0.8</v>
+      </c>
+      <c r="L155">
+        <f t="shared" si="2"/>
+        <v>-5.3000000000000007</v>
+      </c>
+      <c r="M155">
+        <v>0.98</v>
+      </c>
+      <c r="N155">
+        <f t="shared" si="3"/>
+        <v>-2.2206800000000002</v>
+      </c>
+      <c r="O155">
+        <v>-0.25</v>
+      </c>
+      <c r="P155">
+        <f t="shared" si="4"/>
+        <v>-2.4706800000000002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A156" s="2">
+        <v>154</v>
+      </c>
+      <c r="C156" s="2">
+        <v>-1.92384</v>
+      </c>
+      <c r="D156" s="2">
+        <v>-5.0199999999999996</v>
+      </c>
+      <c r="I156">
+        <v>-1.708</v>
+      </c>
+      <c r="J156">
+        <v>-6.2749999999999995</v>
+      </c>
+      <c r="K156">
+        <v>0.8</v>
+      </c>
+      <c r="L156">
+        <f t="shared" si="2"/>
+        <v>-5.0199999999999996</v>
+      </c>
+      <c r="M156">
+        <v>0.98</v>
+      </c>
+      <c r="N156">
+        <f t="shared" si="3"/>
+        <v>-1.67384</v>
+      </c>
+      <c r="O156">
+        <v>-0.25</v>
+      </c>
+      <c r="P156">
+        <f t="shared" si="4"/>
+        <v>-1.92384</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A157" s="2">
+        <v>155</v>
+      </c>
+      <c r="C157" s="2">
+        <v>-1.2986</v>
+      </c>
+      <c r="D157" s="2">
+        <v>-4.66</v>
+      </c>
+      <c r="I157">
+        <v>-1.07</v>
+      </c>
+      <c r="J157">
+        <v>-5.8250000000000002</v>
+      </c>
+      <c r="K157">
+        <v>0.8</v>
+      </c>
+      <c r="L157">
+        <f t="shared" si="2"/>
+        <v>-4.66</v>
+      </c>
+      <c r="M157">
+        <v>0.98</v>
+      </c>
+      <c r="N157">
+        <f t="shared" si="3"/>
+        <v>-1.0486</v>
+      </c>
+      <c r="O157">
+        <v>-0.25</v>
+      </c>
+      <c r="P157">
+        <f t="shared" si="4"/>
+        <v>-1.2986</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A158" s="2">
+        <v>156</v>
+      </c>
+      <c r="C158" s="2">
+        <v>-0.69198000000000004</v>
+      </c>
+      <c r="D158" s="2">
+        <v>-4.68</v>
+      </c>
+      <c r="I158">
+        <v>-0.45100000000000001</v>
+      </c>
+      <c r="J158">
+        <v>-5.85</v>
+      </c>
+      <c r="K158">
+        <v>0.8</v>
+      </c>
+      <c r="L158">
+        <f t="shared" si="2"/>
+        <v>-4.68</v>
+      </c>
+      <c r="M158">
+        <v>0.98</v>
+      </c>
+      <c r="N158">
+        <f t="shared" si="3"/>
+        <v>-0.44197999999999998</v>
+      </c>
+      <c r="O158">
+        <v>-0.25</v>
+      </c>
+      <c r="P158">
+        <f t="shared" si="4"/>
+        <v>-0.69198000000000004</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A159" s="2">
+        <v>157</v>
+      </c>
+      <c r="C159" s="2">
+        <v>-1.6760000000000025E-2</v>
+      </c>
+      <c r="D159" s="2">
+        <v>-4.46</v>
+      </c>
+      <c r="I159">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="J159">
+        <v>-5.5750000000000002</v>
+      </c>
+      <c r="K159">
+        <v>0.8</v>
+      </c>
+      <c r="L159">
+        <f t="shared" si="2"/>
+        <v>-4.46</v>
+      </c>
+      <c r="M159">
+        <v>0.98</v>
+      </c>
+      <c r="N159">
+        <f t="shared" si="3"/>
+        <v>0.23323999999999998</v>
+      </c>
+      <c r="O159">
+        <v>-0.25</v>
+      </c>
+      <c r="P159">
+        <f t="shared" si="4"/>
+        <v>-1.6760000000000025E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A160" s="2">
+        <v>158</v>
+      </c>
+      <c r="C160" s="2">
+        <v>0.70648</v>
+      </c>
+      <c r="D160" s="2">
+        <v>-4.8600000000000003</v>
+      </c>
+      <c r="I160">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="J160">
+        <v>-6.0750000000000002</v>
+      </c>
+      <c r="K160">
+        <v>0.8</v>
+      </c>
+      <c r="L160">
+        <f t="shared" si="2"/>
+        <v>-4.8600000000000003</v>
+      </c>
+      <c r="M160">
+        <v>0.98</v>
+      </c>
+      <c r="N160">
+        <f t="shared" si="3"/>
+        <v>0.95648</v>
+      </c>
+      <c r="O160">
+        <v>-0.25</v>
+      </c>
+      <c r="P160">
+        <f t="shared" si="4"/>
+        <v>0.70648</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A161" s="2">
+        <v>159</v>
+      </c>
+      <c r="C161" s="2">
+        <v>1.4375599999999999</v>
+      </c>
+      <c r="D161" s="2">
+        <v>-5.2</v>
+      </c>
+      <c r="I161">
+        <v>1.722</v>
+      </c>
+      <c r="J161">
+        <v>-6.5</v>
+      </c>
+      <c r="K161">
+        <v>0.8</v>
+      </c>
+      <c r="L161">
+        <f t="shared" si="2"/>
+        <v>-5.2</v>
+      </c>
+      <c r="M161">
+        <v>0.98</v>
+      </c>
+      <c r="N161">
+        <f t="shared" si="3"/>
+        <v>1.6875599999999999</v>
+      </c>
+      <c r="O161">
+        <v>-0.25</v>
+      </c>
+      <c r="P161">
+        <f t="shared" si="4"/>
+        <v>1.4375599999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A162" s="2">
+        <v>160</v>
+      </c>
+      <c r="C162" s="2">
+        <v>2.3273999999999999</v>
+      </c>
+      <c r="D162" s="2">
+        <v>-5.36</v>
+      </c>
+      <c r="I162">
+        <v>2.63</v>
+      </c>
+      <c r="J162">
+        <v>-6.7</v>
+      </c>
+      <c r="K162">
+        <v>0.8</v>
+      </c>
+      <c r="L162">
+        <f t="shared" si="2"/>
+        <v>-5.36</v>
+      </c>
+      <c r="M162">
+        <v>0.98</v>
+      </c>
+      <c r="N162">
+        <f t="shared" si="3"/>
+        <v>2.5773999999999999</v>
+      </c>
+      <c r="O162">
+        <v>-0.25</v>
+      </c>
+      <c r="P162">
+        <f t="shared" si="4"/>
+        <v>2.3273999999999999</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A163" s="2">
+        <v>161</v>
+      </c>
+      <c r="C163" s="2">
+        <v>3.0114400000000003</v>
+      </c>
+      <c r="D163" s="2">
+        <v>-4.9600000000000009</v>
+      </c>
+      <c r="I163">
+        <v>3.3280000000000003</v>
+      </c>
+      <c r="J163">
+        <v>-6.2</v>
+      </c>
+      <c r="K163">
+        <v>0.8</v>
+      </c>
+      <c r="L163">
+        <f t="shared" si="2"/>
+        <v>-4.9600000000000009</v>
+      </c>
+      <c r="M163">
+        <v>0.98</v>
+      </c>
+      <c r="N163">
+        <f t="shared" si="3"/>
+        <v>3.2614400000000003</v>
+      </c>
+      <c r="O163">
+        <v>-0.25</v>
+      </c>
+      <c r="P163">
+        <f t="shared" si="4"/>
+        <v>3.0114400000000003</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A164" s="2">
+        <v>162</v>
+      </c>
+      <c r="C164" s="2">
+        <v>3.6464799999999999</v>
+      </c>
+      <c r="D164" s="2">
+        <v>-4.78</v>
+      </c>
+      <c r="I164">
+        <v>3.976</v>
+      </c>
+      <c r="J164">
+        <v>-5.9750000000000005</v>
+      </c>
+      <c r="K164">
+        <v>0.8</v>
+      </c>
+      <c r="L164">
+        <f t="shared" si="2"/>
+        <v>-4.78</v>
+      </c>
+      <c r="M164">
+        <v>0.98</v>
+      </c>
+      <c r="N164">
+        <f t="shared" si="3"/>
+        <v>3.8964799999999999</v>
+      </c>
+      <c r="O164">
+        <v>-0.25</v>
+      </c>
+      <c r="P164">
+        <f t="shared" si="4"/>
+        <v>3.6464799999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A165" s="2">
+        <v>163</v>
+      </c>
+      <c r="C165" s="2">
+        <v>3.7812299999999999</v>
+      </c>
+      <c r="D165" s="2">
+        <v>-4.88</v>
+      </c>
+      <c r="I165">
+        <v>4.1135000000000002</v>
+      </c>
+      <c r="J165">
+        <v>-6.1</v>
+      </c>
+      <c r="K165">
+        <v>0.8</v>
+      </c>
+      <c r="L165">
+        <f t="shared" si="2"/>
+        <v>-4.88</v>
+      </c>
+      <c r="M165">
+        <v>0.98</v>
+      </c>
+      <c r="N165">
+        <f t="shared" si="3"/>
+        <v>4.0312299999999999</v>
+      </c>
+      <c r="O165">
+        <v>-0.25</v>
+      </c>
+      <c r="P165">
+        <f t="shared" si="4"/>
+        <v>3.7812299999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A166" s="2">
+        <v>164</v>
+      </c>
+      <c r="C166" s="2">
+        <v>4.0620000000000003</v>
+      </c>
+      <c r="D166" s="2">
+        <v>-4.88</v>
+      </c>
+      <c r="I166">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J166">
+        <v>-6.1</v>
+      </c>
+      <c r="K166">
+        <v>0.8</v>
+      </c>
+      <c r="L166">
+        <f t="shared" si="2"/>
+        <v>-4.88</v>
+      </c>
+      <c r="M166">
+        <v>0.98</v>
+      </c>
+      <c r="N166">
+        <f t="shared" si="3"/>
+        <v>4.3120000000000003</v>
+      </c>
+      <c r="O166">
+        <v>-0.25</v>
+      </c>
+      <c r="P166">
+        <f t="shared" si="4"/>
+        <v>4.0620000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18"/>
+  <conditionalFormatting sqref="C2:D31 C47:D166 D32:D46">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{26480379-65DD-4B0F-8FF3-41A50D9C8A51}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32:I46">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{06E9CB48-83CC-4B7B-948F-F932ECEF4613}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{26480379-65DD-4B0F-8FF3-41A50D9C8A51}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C2:D31 C47:D166 D32:D46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{06E9CB48-83CC-4B7B-948F-F932ECEF4613}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H32:I46</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>